<commit_message>
[FIX] missing regression method
</commit_message>
<xml_diff>
--- a/manual/manual-count.xlsx
+++ b/manual/manual-count.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
   <si>
     <t>SUM</t>
   </si>
@@ -70,14 +71,36 @@
   <si>
     <t>c</t>
   </si>
+  <si>
+    <t>X^2</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x*ln(y)</t>
+  </si>
+  <si>
+    <t>x^2</t>
+  </si>
+  <si>
+    <t>y'</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -120,16 +143,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,6 +172,1016 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Y</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.1749999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7869999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.711</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.495000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.904000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.789000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>192.41900000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>336.75</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>589.29999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1800.95</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3157.9870000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5525.7659999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Y'</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$G$3:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0000</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.1789208512254308</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8144639031664012</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6776793936211245</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.690083643726892</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.464902182616623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.826280983781388</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.718228392956149</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109.79582766438264</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>192.21084653374425</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>336.48828294413772</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>589.06334684300248</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1031.2264770642432</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1805.286396951389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3160.371700594626</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5532.6120568936594</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="200864744"/>
+        <c:axId val="200861216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="200864744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="200861216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="200861216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="200864744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7848600" y="104775"/>
+          <a:ext cx="3667125" cy="2809875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 14"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,19 +1447,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q25"/>
+  <dimension ref="B2:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -441,6 +1480,9 @@
       <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="J2" t="s">
         <v>4</v>
       </c>
@@ -459,8 +1501,17 @@
       <c r="O2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
         <v>0.15</v>
       </c>
@@ -483,6 +1534,10 @@
         <f>(E3*F3)</f>
         <v>-2.8518969848491276</v>
       </c>
+      <c r="I3">
+        <f>(C3*C3)</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
       <c r="J3" s="2">
         <v>1</v>
       </c>
@@ -505,10 +1560,17 @@
         <f>(L3*M3)</f>
         <v>0</v>
       </c>
-      <c r="P3" s="2"/>
+      <c r="P3" s="2">
+        <f>(J3*M3)</f>
+        <v>0.77702866454064734</v>
+      </c>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <f>(J3*J3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C4" s="1">
         <v>0.4</v>
       </c>
@@ -516,21 +1578,25 @@
         <v>5.1284000000000001</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E10" si="0">LN(C4)</f>
+        <f t="shared" ref="E4:E9" si="0">LN(C4)</f>
         <v>-0.916290731874155</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" ref="F4:F10" si="1">LN(D4)</f>
+        <f t="shared" ref="F4:F9" si="1">LN(D4)</f>
         <v>1.6347937196964086</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" ref="G4:G10" si="2">(E4*E4)</f>
+        <f t="shared" ref="G4:G9" si="2">(E4*E4)</f>
         <v>0.83958870531847463</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" ref="H4:H9" si="3">(E4*F4)</f>
         <v>-1.4979463338838945</v>
       </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I9" si="4">(C4*C4)</f>
+        <v>0.16000000000000003</v>
+      </c>
       <c r="J4" s="2">
         <v>2</v>
       </c>
@@ -538,25 +1604,32 @@
         <v>3.7869999999999999</v>
       </c>
       <c r="L4" s="6">
-        <f t="shared" ref="L4:M17" si="4">LN(J4)</f>
+        <f t="shared" ref="L4:M17" si="5">LN(J4)</f>
         <v>0.69314718055994529</v>
       </c>
       <c r="M4" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3315741489196578</v>
       </c>
       <c r="N4" s="6">
-        <f t="shared" ref="N4:N17" si="5">(L4*L4)</f>
+        <f t="shared" ref="N4:N17" si="6">(L4*L4)</f>
         <v>0.48045301391820139</v>
       </c>
       <c r="O4" s="6">
-        <f t="shared" ref="O4:O17" si="6">(L4*M4)</f>
+        <f t="shared" ref="O4:O17" si="7">(L4*M4)</f>
         <v>0.92297686703016946</v>
       </c>
-      <c r="P4" s="2"/>
+      <c r="P4" s="2">
+        <f t="shared" ref="P4:P17" si="8">(J4*M4)</f>
+        <v>2.6631482978393155</v>
+      </c>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <f t="shared" ref="R4:R17" si="9">(J4*J4)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>0.6</v>
       </c>
@@ -579,6 +1652,10 @@
         <f t="shared" si="3"/>
         <v>-0.88845597696855516</v>
       </c>
+      <c r="I5">
+        <f t="shared" si="4"/>
+        <v>0.36</v>
+      </c>
       <c r="J5" s="2">
         <v>3</v>
       </c>
@@ -586,25 +1663,32 @@
         <v>6.7</v>
       </c>
       <c r="L5" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0986122886681098</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9021075263969205</v>
       </c>
       <c r="N5" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.2069489608125821</v>
       </c>
       <c r="O5" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.0896787028677579</v>
       </c>
-      <c r="P5" s="2"/>
+      <c r="P5" s="2">
+        <f t="shared" si="8"/>
+        <v>5.7063225791907612</v>
+      </c>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>1.01</v>
       </c>
@@ -627,6 +1711,10 @@
         <f t="shared" si="3"/>
         <v>1.8295739671961207E-2</v>
       </c>
+      <c r="I6">
+        <f t="shared" si="4"/>
+        <v>1.0201</v>
+      </c>
       <c r="J6" s="2">
         <v>4</v>
       </c>
@@ -634,25 +1722,32 @@
         <v>11.711</v>
       </c>
       <c r="L6" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3862943611198906</v>
       </c>
       <c r="M6" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4605285710600002</v>
       </c>
       <c r="N6" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.9218120556728056</v>
       </c>
       <c r="O6" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.4110168834348604</v>
       </c>
-      <c r="P6" s="2"/>
+      <c r="P6" s="2">
+        <f t="shared" si="8"/>
+        <v>9.8421142842400009</v>
+      </c>
       <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>1.5</v>
       </c>
@@ -675,6 +1770,10 @@
         <f t="shared" si="3"/>
         <v>0.79468722011137205</v>
       </c>
+      <c r="I7">
+        <f t="shared" si="4"/>
+        <v>2.25</v>
+      </c>
       <c r="J7" s="2">
         <v>5</v>
       </c>
@@ -682,25 +1781,32 @@
         <v>20.495000000000001</v>
       </c>
       <c r="L7" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6094379124341003</v>
       </c>
       <c r="M7" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.0201809539563009</v>
       </c>
       <c r="N7" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.5902903939802346</v>
       </c>
       <c r="O7" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.8607937297086581</v>
       </c>
-      <c r="P7" s="2"/>
+      <c r="P7" s="2">
+        <f t="shared" si="8"/>
+        <v>15.100904769781504</v>
+      </c>
       <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -723,6 +1829,10 @@
         <f t="shared" si="3"/>
         <v>1.593977154197834</v>
       </c>
+      <c r="I8">
+        <f t="shared" si="4"/>
+        <v>4.8400000000000007</v>
+      </c>
       <c r="J8" s="2">
         <v>6</v>
       </c>
@@ -730,25 +1840,32 @@
         <v>35.904000000000003</v>
       </c>
       <c r="L8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.791759469228055</v>
       </c>
       <c r="M8" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5808487099002311</v>
       </c>
       <c r="N8" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2104019955684011</v>
       </c>
       <c r="O8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.4160195838368033</v>
       </c>
-      <c r="P8" s="2"/>
+      <c r="P8" s="2">
+        <f t="shared" si="8"/>
+        <v>21.485092259401387</v>
+      </c>
       <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <f t="shared" si="9"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>2.4</v>
       </c>
@@ -771,6 +1888,10 @@
         <f t="shared" si="3"/>
         <v>1.765221058877211</v>
       </c>
+      <c r="I9">
+        <f t="shared" si="4"/>
+        <v>5.76</v>
+      </c>
       <c r="J9" s="2">
         <v>7</v>
       </c>
@@ -778,25 +1899,32 @@
         <v>62.789000000000001</v>
       </c>
       <c r="L9" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9459101490553132</v>
       </c>
       <c r="M9" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.1397798988963137</v>
       </c>
       <c r="N9" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7865663081964716</v>
       </c>
       <c r="O9" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8.0556397201175152</v>
       </c>
-      <c r="P9" s="2"/>
+      <c r="P9" s="2">
+        <f t="shared" si="8"/>
+        <v>28.978459292274195</v>
+      </c>
       <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <f t="shared" si="9"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -809,20 +1937,24 @@
         <v>43.766500000000008</v>
       </c>
       <c r="E10" s="8">
-        <f t="shared" ref="E10:H10" si="7">SUM(E3:E9)</f>
+        <f t="shared" ref="E10:H10" si="10">SUM(E3:E9)</f>
         <v>-1.2448948038465244</v>
       </c>
       <c r="F10" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>12.713927850605044</v>
       </c>
       <c r="G10" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>6.2522072424416724</v>
       </c>
       <c r="H10" s="8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1.0661181228431991</v>
+      </c>
+      <c r="I10" s="8">
+        <f t="shared" ref="I10" si="11">SUM(I3:I9)</f>
+        <v>14.412599999999999</v>
       </c>
       <c r="J10" s="2">
         <v>8</v>
@@ -831,25 +1963,32 @@
         <v>109.96</v>
       </c>
       <c r="L10" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.0794415416798357</v>
       </c>
       <c r="M10" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.7001166632970452</v>
       </c>
       <c r="N10" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.3240771252638117</v>
       </c>
       <c r="O10" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.773617840401494</v>
       </c>
-      <c r="P10" s="2"/>
+      <c r="P10" s="2">
+        <f t="shared" si="8"/>
+        <v>37.600933306376362</v>
+      </c>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <f t="shared" si="9"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -858,24 +1997,28 @@
         <v>1.18</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" ref="D11:H11" si="8">AVERAGE(D3:D9)</f>
+        <f t="shared" ref="D11:H11" si="12">AVERAGE(D3:D9)</f>
         <v>6.2523571428571438</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-0.17784211483521778</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1.8162754072292919</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0.89317246320595323</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-0.15230258897759988</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" ref="I11" si="13">AVERAGE(I3:I9)</f>
+        <v>2.0589428571428572</v>
       </c>
       <c r="J11" s="2">
         <v>9</v>
@@ -884,25 +2027,32 @@
         <v>192.41900000000001</v>
       </c>
       <c r="L11" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1972245773362196</v>
       </c>
       <c r="M11" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.2596752859546418</v>
       </c>
       <c r="N11" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.8277958432503283</v>
       </c>
       <c r="O11" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11.556687807107448</v>
       </c>
-      <c r="P11" s="2"/>
+      <c r="P11" s="2">
+        <f t="shared" si="8"/>
+        <v>47.337077573591777</v>
+      </c>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <f t="shared" si="9"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J12" s="2">
         <v>10</v>
       </c>
@@ -910,25 +2060,32 @@
         <v>336.75</v>
       </c>
       <c r="L12" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3025850929940459</v>
       </c>
       <c r="M12" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.8193408152904738</v>
       </c>
       <c r="N12" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.3018981104783993</v>
       </c>
       <c r="O12" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13.399527412339662</v>
       </c>
-      <c r="P12" s="2"/>
+      <c r="P12" s="2">
+        <f t="shared" si="8"/>
+        <v>58.193408152904738</v>
+      </c>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -936,6 +2093,13 @@
         <f>INTERCEPT(F3:F9,E3:E9)</f>
         <v>1.8515132945685935</v>
       </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <f>INTERCEPT(F3:F9,I3:I9)</f>
+        <v>1.6656100127944999</v>
+      </c>
       <c r="J13" s="2">
         <v>11</v>
       </c>
@@ -943,25 +2107,32 @@
         <v>589.29999999999995</v>
       </c>
       <c r="L13" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3978952727983707</v>
       </c>
       <c r="M13" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.3789353918438678</v>
       </c>
       <c r="N13" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.7499017393087728</v>
       </c>
       <c r="O13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15.296019021588632</v>
       </c>
-      <c r="P13" s="2"/>
+      <c r="P13" s="2">
+        <f t="shared" si="8"/>
+        <v>70.168289310282546</v>
+      </c>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <f t="shared" si="9"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -969,6 +2140,9 @@
         <f>(C16-C13)/(C17)</f>
         <v>0.19814140971024627</v>
       </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
       <c r="J14" s="2">
         <v>12</v>
       </c>
@@ -976,25 +2150,32 @@
         <v>1031</v>
       </c>
       <c r="L14" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4849066497880004</v>
       </c>
       <c r="M14" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.9382844840169602</v>
       </c>
       <c r="N14" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.174761058160624</v>
       </c>
       <c r="O14" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17.24098925245465</v>
       </c>
-      <c r="P14" s="2"/>
+      <c r="P14" s="2">
+        <f t="shared" si="8"/>
+        <v>83.259413808203519</v>
+      </c>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <f t="shared" si="9"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -1002,7 +2183,13 @@
         <f>EXP(C13)</f>
         <v>6.3694510888029567</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <f>EXP(F13)</f>
+        <v>5.2888985617114255</v>
+      </c>
       <c r="J15" s="2">
         <v>13</v>
       </c>
@@ -1010,25 +2197,32 @@
         <v>1800.95</v>
       </c>
       <c r="L15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.5649493574615367</v>
       </c>
       <c r="M15" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.496069582436327</v>
       </c>
       <c r="N15" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.5789652063423505</v>
       </c>
       <c r="O15" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>19.227038858957027</v>
       </c>
-      <c r="P15" s="2"/>
+      <c r="P15" s="2">
+        <f t="shared" si="8"/>
+        <v>97.448904571672244</v>
+      </c>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <f t="shared" si="9"/>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
@@ -1036,6 +2230,9 @@
         <f>(F11)</f>
         <v>1.8162754072292919</v>
       </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
       <c r="J16" s="2">
         <v>14</v>
       </c>
@@ -1043,25 +2240,32 @@
         <v>3157.9870000000001</v>
       </c>
       <c r="L16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.6390573296152584</v>
       </c>
       <c r="M16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.0576900782776661</v>
       </c>
       <c r="N16" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.9646235889960186</v>
       </c>
       <c r="O16" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>21.264706060846819</v>
       </c>
-      <c r="P16" s="2"/>
+      <c r="P16" s="2">
+        <f t="shared" si="8"/>
+        <v>112.80766109588733</v>
+      </c>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <f t="shared" si="9"/>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1069,6 +2273,9 @@
         <f>(E11)</f>
         <v>-0.17784211483521778</v>
       </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
       <c r="J17" s="2">
         <v>15</v>
       </c>
@@ -1076,25 +2283,32 @@
         <v>5525.7659999999996</v>
       </c>
       <c r="L17" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7080502011022101</v>
       </c>
       <c r="M17" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.617177159309902</v>
       </c>
       <c r="N17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.3335358916897206</v>
       </c>
       <c r="O17" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>23.335748339202553</v>
       </c>
-      <c r="P17" s="2"/>
+      <c r="P17" s="2">
+        <f t="shared" si="8"/>
+        <v>129.25765738964853</v>
+      </c>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <f t="shared" si="9"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
         <v>0</v>
       </c>
@@ -1107,25 +2321,32 @@
         <v>12887.692999999999</v>
       </c>
       <c r="L18" s="7">
-        <f t="shared" ref="L18:O18" si="9">SUM(L3:L17)</f>
+        <f t="shared" ref="L18:O18" si="14">SUM(L3:L17)</f>
         <v>27.899271383840894</v>
       </c>
       <c r="M18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>70.479337934096961</v>
       </c>
       <c r="N18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>60.452031291638733</v>
       </c>
       <c r="O18" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>156.85046007989405</v>
       </c>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P18" s="7">
+        <f t="shared" ref="P18:R18" si="15">SUM(P3:P17)</f>
+        <v>720.62641535583487</v>
+      </c>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7">
+        <f t="shared" si="15"/>
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>1</v>
       </c>
@@ -1138,25 +2359,32 @@
         <v>859.17953333333332</v>
       </c>
       <c r="L19" s="7">
-        <f t="shared" ref="L19:O19" si="10">AVERAGE(L3:L17)</f>
+        <f t="shared" ref="L19:O19" si="16">AVERAGE(L3:L17)</f>
         <v>1.859951425589393</v>
       </c>
       <c r="M19" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>4.6986225289397971</v>
       </c>
       <c r="N19" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>4.0301354194425825</v>
       </c>
       <c r="O19" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>10.456697338659604</v>
       </c>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="1"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P19" s="7">
+        <f t="shared" ref="P19:R19" si="17">AVERAGE(P3:P17)</f>
+        <v>48.041761023722323</v>
+      </c>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7">
+        <f t="shared" si="17"/>
+        <v>82.666666666666671</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +2393,7 @@
         <v>-0.8986324952863125</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
         <v>9</v>
       </c>
@@ -1174,7 +2402,7 @@
         <v>3.0093554848898361</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
         <v>14</v>
       </c>
@@ -1183,7 +2411,7 @@
         <v>0.407126025996772</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I24" s="4" t="s">
         <v>5</v>
       </c>
@@ -1192,7 +2420,7 @@
         <v>4.6986225289397971</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="I25" s="4" t="s">
         <v>4</v>
       </c>
@@ -1205,4 +2433,734 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="D3" s="10">
+        <f>LN(C3)</f>
+        <v>0.77702866454064734</v>
+      </c>
+      <c r="E3" s="10">
+        <f>(B3*B3)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <f>(B3*D3)</f>
+        <v>0.77702866454064734</v>
+      </c>
+      <c r="G3" s="10">
+        <f>($D$21*$D$22^B3)</f>
+        <v>2.1789208512254308</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" ref="H3:H17" si="0">ABS(C3-G3)</f>
+        <v>3.9208512254309547E-3</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10">
+        <v>3.7869999999999999</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:D17" si="1">LN(C4)</f>
+        <v>1.3315741489196578</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" ref="E4:E17" si="2">(B4*B4)</f>
+        <v>4</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" ref="F4:F17" si="3">(B4*D4)</f>
+        <v>2.6631482978393155</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:I17" si="4">($D$21*$D$22^B4)</f>
+        <v>3.8144639031664012</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="0"/>
+        <v>2.7463903166401238E-2</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10">
+        <v>6.7</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="1"/>
+        <v>1.9021075263969205</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="3"/>
+        <v>5.7063225791907612</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="4"/>
+        <v>6.6776793936211245</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
+        <v>2.2320606378875674E-2</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="10">
+        <v>11.711</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" si="1"/>
+        <v>2.4605285710600002</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="3"/>
+        <v>9.8421142842400009</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="4"/>
+        <v>11.690083643726892</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
+        <v>2.0916356273108505E-2</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10">
+        <v>20.495000000000001</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="1"/>
+        <v>3.0201809539563009</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="3"/>
+        <v>15.100904769781504</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="4"/>
+        <v>20.464902182616623</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="0"/>
+        <v>3.0097817383378356E-2</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10">
+        <v>35.904000000000003</v>
+      </c>
+      <c r="D8" s="10">
+        <f t="shared" si="1"/>
+        <v>3.5808487099002311</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="3"/>
+        <v>21.485092259401387</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="4"/>
+        <v>35.826280983781388</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>7.7719016218615877E-2</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10">
+        <v>62.789000000000001</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" si="1"/>
+        <v>4.1397798988963137</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="3"/>
+        <v>28.978459292274195</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" si="4"/>
+        <v>62.718228392956149</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="0"/>
+        <v>7.0771607043852214E-2</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10">
+        <v>109.96</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="1"/>
+        <v>4.7001166632970452</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" si="3"/>
+        <v>37.600933306376362</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="4"/>
+        <v>109.79582766438264</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="0"/>
+        <v>0.16417233561735145</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
+        <v>9</v>
+      </c>
+      <c r="C11" s="10">
+        <v>192.41900000000001</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="1"/>
+        <v>5.2596752859546418</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" si="3"/>
+        <v>47.337077573591777</v>
+      </c>
+      <c r="G11" s="10">
+        <f t="shared" si="4"/>
+        <v>192.21084653374425</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="0"/>
+        <v>0.20815346625576581</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="10">
+        <v>336.75</v>
+      </c>
+      <c r="D12" s="10">
+        <f t="shared" si="1"/>
+        <v>5.8193408152904738</v>
+      </c>
+      <c r="E12" s="10">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" si="3"/>
+        <v>58.193408152904738</v>
+      </c>
+      <c r="G12" s="10">
+        <f t="shared" si="4"/>
+        <v>336.48828294413772</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.26171705586227745</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
+        <v>11</v>
+      </c>
+      <c r="C13" s="10">
+        <v>589.29999999999995</v>
+      </c>
+      <c r="D13" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3789353918438678</v>
+      </c>
+      <c r="E13" s="10">
+        <f t="shared" si="2"/>
+        <v>121</v>
+      </c>
+      <c r="F13" s="10">
+        <f t="shared" si="3"/>
+        <v>70.168289310282546</v>
+      </c>
+      <c r="G13" s="10">
+        <f t="shared" si="4"/>
+        <v>589.06334684300248</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="0"/>
+        <v>0.2366531569974768</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="12">
+        <v>12</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1031</v>
+      </c>
+      <c r="D14" s="10">
+        <f t="shared" si="1"/>
+        <v>6.9382844840169602</v>
+      </c>
+      <c r="E14" s="10">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+      <c r="F14" s="10">
+        <f t="shared" si="3"/>
+        <v>83.259413808203519</v>
+      </c>
+      <c r="G14" s="10">
+        <f t="shared" si="4"/>
+        <v>1031.2264770642432</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="0"/>
+        <v>0.22647706424322678</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
+        <v>13</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1800.95</v>
+      </c>
+      <c r="D15" s="10">
+        <f t="shared" si="1"/>
+        <v>7.496069582436327</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="3"/>
+        <v>97.448904571672244</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="4"/>
+        <v>1805.286396951389</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="0"/>
+        <v>4.336396951388906</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="12">
+        <v>14</v>
+      </c>
+      <c r="C16" s="10">
+        <v>3157.9870000000001</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" si="1"/>
+        <v>8.0576900782776661</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="2"/>
+        <v>196</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="3"/>
+        <v>112.80766109588733</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="4"/>
+        <v>3160.371700594626</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="0"/>
+        <v>2.3847005946258832</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
+        <v>15</v>
+      </c>
+      <c r="C17" s="10">
+        <v>5525.7659999999996</v>
+      </c>
+      <c r="D17" s="10">
+        <f t="shared" si="1"/>
+        <v>8.617177159309902</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="3"/>
+        <v>129.25765738964853</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="4"/>
+        <v>5532.6120568936594</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="0"/>
+        <v>6.8460568936598065</v>
+      </c>
+      <c r="I17" s="10">
+        <f>($D$21*$D$22^16)</f>
+        <v>9685.5050835716065</v>
+      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="10">
+        <f>SUM(B3:B17)</f>
+        <v>120</v>
+      </c>
+      <c r="C18" s="10">
+        <f t="shared" ref="C18:G18" si="5">SUM(C3:C17)</f>
+        <v>12887.692999999999</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" si="5"/>
+        <v>70.479337934096961</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="5"/>
+        <v>1240</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="5"/>
+        <v>720.62641535583487</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="5"/>
+        <v>12900.425494840278</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" ref="H18" si="6">SUM(H3:H17)</f>
+        <v>14.917537676340357</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="10">
+        <f>AVERAGE(B3:B17)</f>
+        <v>8</v>
+      </c>
+      <c r="C19" s="10">
+        <f t="shared" ref="C19:F19" si="7">AVERAGE(C3:C17)</f>
+        <v>859.17953333333332</v>
+      </c>
+      <c r="D19" s="10">
+        <f t="shared" si="7"/>
+        <v>4.6986225289397971</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" si="7"/>
+        <v>82.666666666666671</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="7"/>
+        <v>48.041761023722323</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" ref="G19" si="8">AVERAGE(G3:G17)</f>
+        <v>860.0283663226852</v>
+      </c>
+      <c r="H19" s="10">
+        <f>AVERAGE(H3:H17)</f>
+        <v>0.99450251175602378</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="10">
+        <f>INTERCEPT(D3:D17,B3:B17)</f>
+        <v>0.21885933228096288</v>
+      </c>
+      <c r="D21" s="9">
+        <f>EXP(C21)</f>
+        <v>1.2446561814266677</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="10">
+        <f>(C24-C21)/C25</f>
+        <v>0.55997039958235428</v>
+      </c>
+      <c r="D22" s="9">
+        <f>EXP(C22)</f>
+        <v>1.7506206804258801</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="10">
+        <f>(D19)</f>
+        <v>4.6986225289397971</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="10">
+        <f>(B19)</f>
+        <v>8</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="11">
+        <f>(G19/C19)*100</f>
+        <v>100.09879576461262</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>